<commit_message>
Modified task sheet answers
</commit_message>
<xml_diff>
--- a/dataset_v1/task_sheet_answers/BoomerangSales/1_BoomerangSales/1_BoomerangSales_gt1.xlsx
+++ b/dataset_v1/task_sheet_answers/BoomerangSales/1_BoomerangSales/1_BoomerangSales_gt1.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12576" windowWidth="23256" xWindow="-108" yWindow="-108"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet2" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Retail Price" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Retail Price" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
   <pivotCaches>
-    <pivotCache xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cacheId="48" r:id="rId4"/>
+    <pivotCache cacheId="48" r:id="rId4"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -21,7 +21,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/d/yy\ hh:mm"/>
+    <numFmt formatCode="m/d/yy\ hh:mm" numFmtId="164"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -86,37 +86,37 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="1" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="1" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -189,7 +189,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <pivotSource>
     <name>[1_BoomerangSales.xlsx]Sheet2!PivotTable15</name>
     <fmtId val="0"/>
@@ -198,11 +198,11 @@
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr anchor="ctr" anchorCtr="1" rot="0" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr b="0" baseline="0" i="0" kern="1200" spc="0" strike="noStrike" sz="1400">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -215,7 +215,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:rPr altLang="zh-CN" lang="en-US"/>
               <a:t>Sales frequency by website</a:t>
             </a:r>
           </a:p>
@@ -223,18 +223,18 @@
       </tx>
       <overlay val="0"/>
       <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
       <txPr>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:bodyPr anchor="ctr" anchorCtr="1" rot="0" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
+        <a:lstStyle/>
+        <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr b="0" baseline="0" i="0" kern="1200" spc="0" strike="noStrike" sz="1400">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -247,7 +247,7 @@
             </a:defRPr>
           </a:pPr>
           <a:r>
-            <a:t/>
+            <a:t>None</a:t>
           </a:r>
           <a:endParaRPr lang="zh-CN"/>
         </a:p>
@@ -257,10 +257,10 @@
       <pivotFmt>
         <idx val="0"/>
         <spPr>
-          <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
-          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:ln>
             <a:noFill/>
             <a:prstDash val="solid"/>
           </a:ln>
@@ -268,7 +268,7 @@
         <marker>
           <symbol val="none"/>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
@@ -276,20 +276,20 @@
         <dLbl>
           <idx val="0"/>
           <spPr>
-            <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:noFill/>
+            <a:ln>
               <a:noFill/>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <txPr>
-            <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+            <a:bodyPr anchor="ctr" anchorCtr="1" bIns="19050" lIns="38100" rIns="38100" rot="0" spcFirstLastPara="1" tIns="19050" vert="horz" vertOverflow="ellipsis" wrap="square">
               <a:spAutoFit/>
             </a:bodyPr>
-            <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-            <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:lstStyle/>
+            <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr b="0" baseline="0" i="0" kern="1200" strike="noStrike" sz="900">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="75000"/>
@@ -302,7 +302,7 @@
                 </a:defRPr>
               </a:pPr>
               <a:r>
-                <a:t/>
+                <a:t>None</a:t>
               </a:r>
               <a:endParaRPr lang="zh-CN"/>
             </a:p>
@@ -337,10 +337,10 @@
             </strRef>
           </tx>
           <spPr>
-            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:solidFill>
               <a:schemeClr val="accent1"/>
             </a:solidFill>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:noFill/>
               <a:prstDash val="solid"/>
             </a:ln>
@@ -412,8 +412,8 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
             <a:solidFill>
               <a:schemeClr val="tx1">
                 <a:lumMod val="15000"/>
@@ -425,11 +425,11 @@
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr anchor="ctr" anchorCtr="1" rot="-60000000" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr b="0" baseline="0" i="0" kern="1200" strike="noStrike" sz="900">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -442,7 +442,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
@@ -463,7 +463,7 @@
         <axPos val="b"/>
         <majorGridlines>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="15000"/>
@@ -480,18 +480,18 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:noFill/>
+          <a:ln>
             <a:noFill/>
             <a:prstDash val="solid"/>
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr anchor="ctr" anchorCtr="1" rot="-60000000" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr b="0" baseline="0" i="0" kern="1200" strike="noStrike" sz="900">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -504,7 +504,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
@@ -517,26 +517,11 @@
     <plotVisOnly val="1"/>
     <dispBlanksAs val="gap"/>
   </chart>
-  <spPr>
-    <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:prstDash val="solid"/>
-      <a:round/>
-    </a:ln>
-  </spPr>
 </chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <twoCellAnchor>
     <from>
       <col>2</col>
@@ -556,9 +541,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -568,15 +553,15 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" refreshedBy="hongxin li" refreshedDate="45055.64457719908" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="35" r:id="rId1">
+<pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" createdVersion="8" minRefreshableVersion="3" recordCount="35" refreshedBy="hongxin li" refreshedDate="45055.64457719908" refreshedVersion="8" r:id="rId1">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:G36" sheet="Sheet1"/>
   </cacheSource>
   <cacheFields count="7">
-    <cacheField name="Date Time" uniqueList="1" numFmtId="176" sqlType="0" hierarchy="0" level="0" databaseField="1">
-      <sharedItems count="0" containsDate="1" containsNonDate="0" containsSemiMixedTypes="0" containsString="0" minDate="2014-12-06T17:46:02" maxDate="2015-12-20T12:35:00"/>
+    <cacheField databaseField="1" hierarchy="0" level="0" name="Date Time" numFmtId="176" sqlType="0" uniqueList="1">
+      <sharedItems containsDate="1" containsNonDate="0" containsSemiMixedTypes="0" containsString="0" count="0" maxDate="2015-12-20T12:35:00" minDate="2014-12-06T17:46:02"/>
     </cacheField>
-    <cacheField name="Web Site" uniqueList="1" numFmtId="0" sqlType="0" hierarchy="0" level="0" databaseField="1">
+    <cacheField databaseField="1" hierarchy="0" level="0" name="Web Site" numFmtId="0" sqlType="0" uniqueList="1">
       <sharedItems count="4">
         <s v="amazon.com"/>
         <s v="ebay.com"/>
@@ -584,20 +569,20 @@
         <s v="gel-boomerang.com"/>
       </sharedItems>
     </cacheField>
-    <cacheField name="Product" uniqueList="1" numFmtId="0" sqlType="0" hierarchy="0" level="0" databaseField="1">
+    <cacheField databaseField="1" hierarchy="0" level="0" name="Product" numFmtId="0" sqlType="0" uniqueList="1">
       <sharedItems count="0"/>
     </cacheField>
-    <cacheField name="Type" uniqueList="1" numFmtId="0" sqlType="0" hierarchy="0" level="0" databaseField="1">
+    <cacheField databaseField="1" hierarchy="0" level="0" name="Type" numFmtId="0" sqlType="0" uniqueList="1">
       <sharedItems count="0"/>
     </cacheField>
-    <cacheField name="Quantity" uniqueList="1" numFmtId="0" sqlType="0" hierarchy="0" level="0" databaseField="1">
-      <sharedItems count="0" containsInteger="1" containsNumber="1" containsSemiMixedTypes="0" containsString="0" minValue="1" maxValue="124"/>
+    <cacheField databaseField="1" hierarchy="0" level="0" name="Quantity" numFmtId="0" sqlType="0" uniqueList="1">
+      <sharedItems containsInteger="1" containsNumber="1" containsSemiMixedTypes="0" containsString="0" count="0" maxValue="124" minValue="1"/>
     </cacheField>
-    <cacheField name="Discount" uniqueList="1" numFmtId="0" sqlType="0" hierarchy="0" level="0" databaseField="1">
-      <sharedItems count="0" containsNumber="1" containsSemiMixedTypes="0" containsString="0" minValue="0" maxValue="0.594"/>
+    <cacheField databaseField="1" hierarchy="0" level="0" name="Discount" numFmtId="0" sqlType="0" uniqueList="1">
+      <sharedItems containsNumber="1" containsSemiMixedTypes="0" containsString="0" count="0" maxValue="0.594" minValue="0"/>
     </cacheField>
-    <cacheField name="Revenue" uniqueList="1" numFmtId="0" sqlType="0" hierarchy="0" level="0" databaseField="1">
-      <sharedItems count="0" containsNumber="1" containsSemiMixedTypes="0" containsString="0" minValue="4.905" maxValue="2011.2428"/>
+    <cacheField databaseField="1" hierarchy="0" level="0" name="Revenue" numFmtId="0" sqlType="0" uniqueList="1">
+      <sharedItems containsNumber="1" containsSemiMixedTypes="0" containsString="0" count="0" maxValue="2011.2428" minValue="4.905"/>
     </cacheField>
   </cacheFields>
 </pivotCacheDefinition>
@@ -924,54 +909,54 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable15" cacheId="48" dataOnRows="0" dataCaption="Values" showError="0" showMissing="1" updatedVersion="8" minRefreshableVersion="3" asteriskTotals="0" showItems="1" editData="0" disableFieldList="0" showCalcMbrs="1" visualTotals="1" showMultipleLabel="1" showDataDropDown="1" showDrill="1" printDrill="0" showMemberPropertyTips="1" showDataTips="1" enableWizard="1" enableDrill="1" enableFieldProperties="1" preserveFormatting="1" useAutoFormatting="1" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" rowGrandTotals="1" colGrandTotals="1" fieldPrintTitles="0" itemPrintTitles="1" mergeItem="0" showDropZones="1" createdVersion="8" indent="0" showEmptyRow="0" showEmptyCol="0" showHeaders="1" compact="1" outline="1" outlineData="1" compactData="1" published="0" gridDropZones="0" immersive="1" multipleFieldFilters="0" chartFormat="1" fieldListSortAscending="0" mdxSubqueries="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" r:id="rId1">
-  <location ref="A1:B6" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" applyAlignmentFormats="0" applyBorderFormats="0" applyFontFormats="0" applyNumberFormats="0" applyPatternFormats="0" applyWidthHeightFormats="1" asteriskTotals="0" cacheId="48" chartFormat="1" colGrandTotals="1" compact="1" compactData="1" createdVersion="8" dataCaption="Values" dataOnRows="0" disableFieldList="0" editData="0" enableDrill="1" enableFieldProperties="1" enableWizard="1" fieldListSortAscending="0" fieldPrintTitles="0" gridDropZones="0" immersive="1" indent="0" itemPrintTitles="1" mdxSubqueries="0" mergeItem="0" minRefreshableVersion="3" multipleFieldFilters="0" name="PivotTable15" outline="1" outlineData="1" pageOverThenDown="0" pageWrap="0" preserveFormatting="1" printDrill="0" published="0" rowGrandTotals="1" showCalcMbrs="1" showDataDropDown="1" showDataTips="1" showDrill="1" showDropZones="1" showEmptyCol="0" showEmptyRow="0" showError="0" showHeaders="1" showItems="1" showMemberPropertyTips="1" showMissing="1" showMultipleLabel="1" subtotalHiddenItems="0" updatedVersion="8" useAutoFormatting="1" visualTotals="1" r:id="rId1">
+  <location firstDataCol="1" firstDataRow="1" firstHeaderRow="1" ref="A1:B6"/>
   <pivotFields count="7">
-    <pivotField showDropDowns="1" compact="1" numFmtId="176" outline="1" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1"/>
-    <pivotField axis="axisRow" showDropDowns="1" compact="1" outline="1" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1">
+    <pivotField compact="1" defaultSubtotal="1" dragOff="1" dragToCol="1" dragToData="1" dragToPage="1" dragToRow="1" itemPageCount="10" numFmtId="176" outline="1" showAll="0" showDropDowns="1" sortType="manual" subtotalTop="1" topAutoShow="1"/>
+    <pivotField axis="axisRow" compact="1" defaultSubtotal="1" dragOff="1" dragToCol="1" dragToData="1" dragToPage="1" dragToRow="1" itemPageCount="10" outline="1" showAll="0" showDropDowns="1" sortType="manual" subtotalTop="1" topAutoShow="1">
       <items count="5">
-        <item t="data" sd="1" x="0"/>
-        <item t="data" sd="1" x="2"/>
-        <item t="data" sd="1" x="1"/>
-        <item t="data" sd="1" x="3"/>
-        <item t="default" sd="1"/>
+        <item sd="1" t="data" x="0"/>
+        <item sd="1" t="data" x="2"/>
+        <item sd="1" t="data" x="1"/>
+        <item sd="1" t="data" x="3"/>
+        <item sd="1" t="default"/>
       </items>
     </pivotField>
-    <pivotField showDropDowns="1" compact="1" outline="1" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1"/>
-    <pivotField showDropDowns="1" compact="1" outline="1" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1"/>
-    <pivotField showDropDowns="1" compact="1" outline="1" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1"/>
-    <pivotField showDropDowns="1" compact="1" outline="1" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1"/>
-    <pivotField dataField="1" showDropDowns="1" compact="1" outline="1" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1"/>
+    <pivotField compact="1" defaultSubtotal="1" dragOff="1" dragToCol="1" dragToData="1" dragToPage="1" dragToRow="1" itemPageCount="10" outline="1" showAll="0" showDropDowns="1" sortType="manual" subtotalTop="1" topAutoShow="1"/>
+    <pivotField compact="1" defaultSubtotal="1" dragOff="1" dragToCol="1" dragToData="1" dragToPage="1" dragToRow="1" itemPageCount="10" outline="1" showAll="0" showDropDowns="1" sortType="manual" subtotalTop="1" topAutoShow="1"/>
+    <pivotField compact="1" defaultSubtotal="1" dragOff="1" dragToCol="1" dragToData="1" dragToPage="1" dragToRow="1" itemPageCount="10" outline="1" showAll="0" showDropDowns="1" sortType="manual" subtotalTop="1" topAutoShow="1"/>
+    <pivotField compact="1" defaultSubtotal="1" dragOff="1" dragToCol="1" dragToData="1" dragToPage="1" dragToRow="1" itemPageCount="10" outline="1" showAll="0" showDropDowns="1" sortType="manual" subtotalTop="1" topAutoShow="1"/>
+    <pivotField compact="1" dataField="1" defaultSubtotal="1" dragOff="1" dragToCol="1" dragToData="1" dragToPage="1" dragToRow="1" itemPageCount="10" outline="1" showAll="0" showDropDowns="1" sortType="manual" subtotalTop="1" topAutoShow="1"/>
   </pivotFields>
   <rowFields count="1">
     <field x="1"/>
   </rowFields>
   <rowItems count="5">
-    <i t="data" r="0" i="0">
+    <i i="0" r="0" t="data">
       <x v="0"/>
     </i>
-    <i t="data" r="0" i="0">
+    <i i="0" r="0" t="data">
       <x v="1"/>
     </i>
-    <i t="data" r="0" i="0">
+    <i i="0" r="0" t="data">
       <x v="2"/>
     </i>
-    <i t="data" r="0" i="0">
+    <i i="0" r="0" t="data">
       <x v="3"/>
     </i>
-    <i t="grand" r="0" i="0">
+    <i i="0" r="0" t="grand">
       <x v="0"/>
     </i>
   </rowItems>
   <colItems count="1">
-    <i t="data" r="0" i="0"/>
+    <i i="0" r="0" t="data"/>
   </colItems>
   <dataFields count="1">
-    <dataField name="Count of Revenue" fld="6" subtotal="count" showDataAs="normal" baseField="1" baseItem="0"/>
+    <dataField baseField="1" baseItem="0" fld="6" name="Count of Revenue" showDataAs="normal" subtotal="count"/>
   </dataFields>
   <chartFormats count="1">
     <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" dataOnly="1" outline="0" fieldPosition="0">
+      <pivotArea dataOnly="1" fieldPosition="0" outline="0" type="data">
         <references count="1">
           <reference field="4294967294" selected="0">
             <x v="0"/>
@@ -980,7 +965,7 @@
       </pivotArea>
     </chartFormat>
   </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <pivotTableStyleInfo name="PivotStyleLight16" showColHeaders="1" showColStripes="0" showLastColumn="1" showRowHeaders="1" showRowStripes="0"/>
 </pivotTableDefinition>
 </file>
 
@@ -1280,7 +1265,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -1293,8 +1278,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8"/>
   <cols>
-    <col width="25.109375" bestFit="1" customWidth="1" style="7" min="1" max="1"/>
-    <col width="19" bestFit="1" customWidth="1" style="7" min="2" max="2"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" style="7" width="25.109375"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" style="7" width="19"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1360,8 +1345,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1379,7 +1364,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
   <cols>
-    <col width="13.77734375" customWidth="1" style="8" min="1" max="1"/>
+    <col customWidth="1" max="1" min="1" style="8" width="13.77734375"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2435,7 +2420,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
@@ -2453,8 +2438,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
   <cols>
-    <col width="16.109375" customWidth="1" style="7" min="1" max="1"/>
-    <col width="12.77734375" customWidth="1" style="7" min="2" max="2"/>
+    <col customWidth="1" max="1" min="1" style="7" width="16.109375"/>
+    <col customWidth="1" max="2" min="2" style="7" width="12.77734375"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2690,6 +2675,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>